<commit_message>
Updated with UVa Data - take 2.
</commit_message>
<xml_diff>
--- a/data/UNCCH-tuition.xlsx
+++ b/data/UNCCH-tuition.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="0" windowWidth="25360" windowHeight="14860" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="40" yWindow="0" windowWidth="25500" windowHeight="14860" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="97">
   <si>
     <t>1947-1948</t>
   </si>
@@ -311,12 +311,6 @@
   </si>
   <si>
     <t>Enrollment %</t>
-  </si>
-  <si>
-    <t>University of Virginia</t>
-  </si>
-  <si>
-    <t>All Students</t>
   </si>
 </sst>
 </file>
@@ -4440,8 +4434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW34"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AL27" sqref="AL27"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6881,59 +6875,29 @@
       <c r="O28" s="26"/>
     </row>
     <row r="30" spans="1:47" ht="16">
-      <c r="E30" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="F30" s="32">
-        <v>2001</v>
-      </c>
-      <c r="G30" s="32" t="s">
-        <v>98</v>
-      </c>
+      <c r="E30" s="31"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
     </row>
     <row r="31" spans="1:47" ht="16">
-      <c r="E31" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="F31" s="32">
-        <v>2002</v>
-      </c>
-      <c r="G31" s="32" t="s">
-        <v>98</v>
-      </c>
+      <c r="E31" s="31"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
     </row>
     <row r="32" spans="1:47" ht="16">
-      <c r="E32" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="F32" s="32">
-        <v>2003</v>
-      </c>
-      <c r="G32" s="32" t="s">
-        <v>98</v>
-      </c>
+      <c r="E32" s="31"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
     </row>
     <row r="33" spans="5:7" ht="16">
-      <c r="E33" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="F33" s="32">
-        <v>2004</v>
-      </c>
-      <c r="G33" s="32" t="s">
-        <v>98</v>
-      </c>
+      <c r="E33" s="31"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
     </row>
     <row r="34" spans="5:7" ht="16">
-      <c r="E34" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="F34" s="32">
-        <v>2005</v>
-      </c>
-      <c r="G34" s="32" t="s">
-        <v>98</v>
-      </c>
+      <c r="E34" s="31"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="26">
@@ -6964,13 +6928,6 @@
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="T2:U2"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="E30" r:id="rId1"/>
-    <hyperlink ref="E31" r:id="rId2"/>
-    <hyperlink ref="E32" r:id="rId3"/>
-    <hyperlink ref="E33" r:id="rId4"/>
-    <hyperlink ref="E34" r:id="rId5"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Added images, produced C3 graphics and beginning legacy tuition feature.
</commit_message>
<xml_diff>
--- a/data/UNCCH-tuition.xlsx
+++ b/data/UNCCH-tuition.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pchance2/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40" yWindow="0" windowWidth="25500" windowHeight="14860" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1980" yWindow="3280" windowWidth="49520" windowHeight="26740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -20,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="99">
   <si>
     <t>1947-1948</t>
   </si>
@@ -311,6 +319,12 @@
   </si>
   <si>
     <t>Enrollment %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of Enrollment </t>
+  </si>
+  <si>
+    <t>Percentage of Tuition Revenue</t>
   </si>
 </sst>
 </file>
@@ -318,10 +332,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -430,71 +451,71 @@
   </borders>
   <cellStyleXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -509,18 +530,26 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="5" borderId="0" xfId="46" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="4" borderId="0" xfId="46" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="46" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="46" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="59"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -529,23 +558,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="6" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="59"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="62">
     <cellStyle name="Comma" xfId="46" builtinId="3"/>
@@ -613,6 +635,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1556,22 +1583,22 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127999784"/>
-        <c:axId val="2127996792"/>
+        <c:axId val="1576444608"/>
+        <c:axId val="1612615568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127999784"/>
+        <c:axId val="1576444608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127996792"/>
+        <c:crossAx val="1612615568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1579,7 +1606,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127996792"/>
+        <c:axId val="1612615568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1590,13 +1617,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127999784"/>
+        <c:crossAx val="1576444608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1609,6 +1637,2120 @@
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Percentage of Total Undergraguate Population from Out of State</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$W$31:$W$32</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Percentage of Enrollment </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>UNC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$W$33:$W$44</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.174783928988554</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.176707510778307</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.174853310980721</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.174795617596352</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.186662360729856</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.191915355398806</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.194671134410636</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.192270005443658</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.193024523160763</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.192451805593266</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.187388651946229</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.178931184391899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$X$31:$X$32</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Percentage of Enrollment </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>UVA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$X$33:$X$44</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.297333427144164</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.331698010357045</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.329420347526197</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.33359637009272</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.341044197467046</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.335043283103559</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.328004060398427</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.335229427379598</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.331468357578018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.331371716313778</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.328752390057361</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.304329189884269</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$Y$31:$Y$32</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Percentage of Enrollment </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Berkeley</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$Y$33:$Y$44</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.0945830849161059</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0880023467292461</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0873112518265952</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0924018925688839</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.101449275362319</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.126664056382146</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.168746378211319</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.19193761154652</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.233748217795075</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.241613212416132</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.244253709630492</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.243858332195987</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1724786176"/>
+        <c:axId val="1724282592"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1724786176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1724282592"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1724282592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1724786176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Percentage of Total Tuition Revenue</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Generate by Out-of-State Students</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$AX$28:$AX$29</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Percentage of Tuition Revenue</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>UNC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$AX$30:$AX$41</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.458092342278346</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.456317109479905</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.454404873138528</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.466675847471158</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.489623393875792</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.47390653258829</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.480643584569066</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.468197732001741</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.463494212654262</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.490294381570136</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.474749760566722</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.455508026261416</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$AY$28:$AY$29</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Percentage of Tuition Revenue</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>UVA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$AY$30:$AY$41</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.586831961554626</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.62142177664071</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.61594260376646</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.610971160358568</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.625467773860333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.611017671784923</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.603568067541653</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.61200533861594</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.610441028420086</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.613910464285981</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.594609133895886</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.554206328862783</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$AZ$28:$AZ$29</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Percentage of Tuition Revenue</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Berkeley</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$AZ$30:$AZ$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.261925069168823</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.246789002523802</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.242171717585949</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25189891935541</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.265304367221101</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.291440902808585</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.343906405430386</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.375061233547191</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.432962575399429</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.440864793751977</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.447817132411741</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.457832375151591</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1804193472"/>
+        <c:axId val="1804195520"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1804193472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1804195520"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1804195520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1804193472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1638,6 +3780,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1970,11 +4177,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O73"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="T3" workbookViewId="0">
-      <selection activeCell="A57" sqref="A3:XFD57"/>
+    <sheetView showRuler="0" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.83203125" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
@@ -1988,7 +4195,7 @@
     <col min="15" max="15" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -2035,7 +4242,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2062,7 +4269,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2089,7 +4296,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -2116,7 +4323,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2143,7 +4350,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2170,7 +4377,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2197,7 +4404,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -2224,7 +4431,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -2251,7 +4458,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2278,7 +4485,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -2305,7 +4512,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -2332,7 +4539,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -2359,7 +4566,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -2386,7 +4593,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2413,7 +4620,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2440,7 +4647,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2467,7 +4674,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2494,7 +4701,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -2521,7 +4728,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2548,7 +4755,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2575,7 +4782,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2602,7 +4809,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -2629,7 +4836,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2656,7 +4863,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -2683,7 +4890,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2710,7 +4917,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -2737,7 +4944,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -2764,7 +4971,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -2791,7 +4998,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -2818,7 +5025,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -2845,7 +5052,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -2872,7 +5079,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -2899,7 +5106,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -2926,7 +5133,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -2953,7 +5160,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -2980,7 +5187,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -3007,7 +5214,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -3034,7 +5241,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>37</v>
       </c>
@@ -3061,7 +5268,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>38</v>
       </c>
@@ -3088,7 +5295,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>39</v>
       </c>
@@ -3115,7 +5322,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>40</v>
       </c>
@@ -3142,7 +5349,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>41</v>
       </c>
@@ -3169,7 +5376,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -3196,7 +5403,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>43</v>
       </c>
@@ -3223,7 +5430,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>44</v>
       </c>
@@ -3250,7 +5457,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -3277,7 +5484,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>46</v>
       </c>
@@ -3304,7 +5511,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>47</v>
       </c>
@@ -3331,7 +5538,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -3358,7 +5565,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>49</v>
       </c>
@@ -3385,7 +5592,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>50</v>
       </c>
@@ -3412,7 +5619,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>51</v>
       </c>
@@ -3439,7 +5646,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>52</v>
       </c>
@@ -3466,7 +5673,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>53</v>
       </c>
@@ -3522,7 +5729,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>54</v>
       </c>
@@ -3578,7 +5785,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>55</v>
       </c>
@@ -3634,7 +5841,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>56</v>
       </c>
@@ -3690,7 +5897,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>57</v>
       </c>
@@ -3746,7 +5953,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>58</v>
       </c>
@@ -3802,7 +6009,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>59</v>
       </c>
@@ -3858,7 +6065,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>60</v>
       </c>
@@ -3914,7 +6121,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>61</v>
       </c>
@@ -3970,7 +6177,7 @@
         <v>1692</v>
       </c>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>62</v>
       </c>
@@ -4026,7 +6233,7 @@
         <v>1760</v>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>63</v>
       </c>
@@ -4082,7 +6289,7 @@
         <v>1850</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>64</v>
       </c>
@@ -4138,7 +6345,7 @@
         <v>1881</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>65</v>
       </c>
@@ -4194,7 +6401,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>66</v>
       </c>
@@ -4250,7 +6457,7 @@
         <v>1917</v>
       </c>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>67</v>
       </c>
@@ -4306,7 +6513,7 @@
         <v>1923</v>
       </c>
     </row>
-    <row r="72" spans="1:15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>68</v>
       </c>
@@ -4362,7 +6569,7 @@
         <v>1943</v>
       </c>
     </row>
-    <row r="73" spans="1:15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>69</v>
       </c>
@@ -4422,30 +6629,25 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW34"/>
+  <dimension ref="A1:AZ44"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AD20" sqref="AD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="7" width="10.83203125" customWidth="1"/>
     <col min="11" max="13" width="0" hidden="1" customWidth="1"/>
     <col min="16" max="17" width="10.83203125" customWidth="1"/>
     <col min="20" max="21" width="0" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.1640625" customWidth="1"/>
+    <col min="23" max="23" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12.5" customWidth="1"/>
     <col min="25" max="27" width="10.83203125" customWidth="1"/>
     <col min="28" max="28" width="15.1640625" bestFit="1" customWidth="1"/>
@@ -4456,164 +6658,165 @@
     <col min="40" max="41" width="0" hidden="1" customWidth="1"/>
     <col min="44" max="45" width="10.83203125" customWidth="1"/>
     <col min="48" max="49" width="0" hidden="1" customWidth="1"/>
+    <col min="50" max="50" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="19" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="20" t="s">
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="20"/>
-      <c r="AG1" s="20"/>
-      <c r="AH1" s="19" t="s">
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="AI1" s="19"/>
-      <c r="AJ1" s="19"/>
-      <c r="AK1" s="19"/>
-      <c r="AL1" s="19"/>
-      <c r="AM1" s="19"/>
-      <c r="AN1" s="19"/>
-      <c r="AO1" s="19"/>
-      <c r="AP1" s="20" t="s">
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="AQ1" s="20"/>
-      <c r="AR1" s="20"/>
-      <c r="AS1" s="20"/>
-      <c r="AT1" s="20"/>
-      <c r="AU1" s="20"/>
-      <c r="AV1" s="20"/>
-      <c r="AW1" s="20"/>
-    </row>
-    <row r="2" spans="1:49">
-      <c r="A2" s="22"/>
-      <c r="B2" s="21" t="s">
+      <c r="AQ1" s="28"/>
+      <c r="AR1" s="28"/>
+      <c r="AS1" s="28"/>
+      <c r="AT1" s="28"/>
+      <c r="AU1" s="28"/>
+      <c r="AV1" s="28"/>
+      <c r="AW1" s="28"/>
+    </row>
+    <row r="2" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A2" s="27"/>
+      <c r="B2" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="24" t="s">
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="23" t="s">
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="22" t="s">
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="21" t="s">
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="O2" s="21"/>
-      <c r="P2" s="22" t="s">
+      <c r="O2" s="29"/>
+      <c r="P2" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="23" t="s">
+      <c r="Q2" s="27"/>
+      <c r="R2" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="S2" s="23"/>
-      <c r="T2" s="22" t="s">
+      <c r="S2" s="30"/>
+      <c r="T2" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="U2" s="22"/>
-      <c r="V2" s="21" t="s">
+      <c r="U2" s="27"/>
+      <c r="V2" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="22" t="s">
+      <c r="W2" s="29"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="23" t="s">
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="AC2" s="23"/>
-      <c r="AD2" s="23"/>
-      <c r="AE2" s="22" t="s">
+      <c r="AC2" s="30"/>
+      <c r="AD2" s="30"/>
+      <c r="AE2" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="AF2" s="22"/>
-      <c r="AG2" s="22"/>
-      <c r="AH2" s="21" t="s">
+      <c r="AF2" s="27"/>
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="AI2" s="21"/>
-      <c r="AJ2" s="22" t="s">
+      <c r="AI2" s="29"/>
+      <c r="AJ2" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="AK2" s="22"/>
-      <c r="AL2" s="23" t="s">
+      <c r="AK2" s="27"/>
+      <c r="AL2" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="AM2" s="23"/>
-      <c r="AN2" s="22" t="s">
+      <c r="AM2" s="30"/>
+      <c r="AN2" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="AO2" s="22"/>
-      <c r="AP2" s="21" t="s">
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="AQ2" s="21"/>
-      <c r="AR2" s="22" t="s">
+      <c r="AQ2" s="29"/>
+      <c r="AR2" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="AS2" s="22"/>
-      <c r="AT2" s="23" t="s">
+      <c r="AS2" s="27"/>
+      <c r="AT2" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="AU2" s="23"/>
-      <c r="AV2" s="22" t="s">
+      <c r="AU2" s="30"/>
+      <c r="AV2" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="AW2" s="22"/>
-    </row>
-    <row r="3" spans="1:49">
-      <c r="A3" s="22"/>
+      <c r="AW2" s="27"/>
+    </row>
+    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A3" s="27"/>
       <c r="B3" s="18" t="s">
         <v>89</v>
       </c>
@@ -4759,7 +6962,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:49" ht="17">
+    <row r="4" spans="1:49" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -4773,13 +6976,13 @@
         <f>B4+C4</f>
         <v>15844</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="24">
         <v>9367</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="24">
         <v>4345</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="24">
         <v>13712</v>
       </c>
       <c r="H4" s="6">
@@ -4798,7 +7001,7 @@
       <c r="O4" s="10">
         <v>11934</v>
       </c>
-      <c r="P4" s="25"/>
+      <c r="P4" s="19"/>
       <c r="R4" s="11">
         <v>4046.5</v>
       </c>
@@ -4865,7 +7068,7 @@
         <v>0.117779345621307</v>
       </c>
     </row>
-    <row r="5" spans="1:49" ht="16">
+    <row r="5" spans="1:49" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -4879,13 +7082,13 @@
         <f t="shared" ref="D5:D20" si="0">B5+C5</f>
         <v>15961</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="24">
         <v>9493</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="24">
         <v>4271</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="24">
         <v>13764</v>
       </c>
       <c r="H5" s="6">
@@ -4971,7 +7174,7 @@
         <v>0.11607718423653789</v>
       </c>
     </row>
-    <row r="6" spans="1:49" ht="16">
+    <row r="6" spans="1:49" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -4985,13 +7188,13 @@
         <f t="shared" si="0"/>
         <v>16144</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="24">
         <v>9606</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="24">
         <v>4199</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="24">
         <v>13805</v>
       </c>
       <c r="H6" s="6">
@@ -5077,7 +7280,7 @@
         <v>0.10589469267883365</v>
       </c>
     </row>
-    <row r="7" spans="1:49" ht="16">
+    <row r="7" spans="1:49" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -5091,13 +7294,13 @@
         <f t="shared" si="0"/>
         <v>16525</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="24">
         <v>9543</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="24">
         <v>4286</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="24">
         <v>13829</v>
       </c>
       <c r="H7" s="6">
@@ -5181,7 +7384,7 @@
         <v>0.10363699043350857</v>
       </c>
     </row>
-    <row r="8" spans="1:49" ht="16">
+    <row r="8" spans="1:49" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -5195,13 +7398,13 @@
         <f t="shared" si="0"/>
         <v>16764</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="24">
         <v>9709</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="24">
         <v>4420</v>
       </c>
-      <c r="G8" s="30">
+      <c r="G8" s="24">
         <v>14129</v>
       </c>
       <c r="H8" s="6">
@@ -5287,7 +7490,7 @@
         <v>9.9781468531468534E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:49" ht="16">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -5301,13 +7504,13 @@
         <f t="shared" si="0"/>
         <v>17124</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="24">
         <v>9987</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="24">
         <v>4226</v>
       </c>
-      <c r="G9" s="30">
+      <c r="G9" s="24">
         <v>14213</v>
       </c>
       <c r="H9" s="6">
@@ -5326,10 +7529,10 @@
       <c r="O9" s="10">
         <v>18411</v>
       </c>
-      <c r="P9" s="28">
+      <c r="P9" s="22">
         <v>7180</v>
       </c>
-      <c r="Q9" s="29">
+      <c r="Q9" s="23">
         <v>24100</v>
       </c>
       <c r="R9" s="11">
@@ -5419,7 +7622,7 @@
         <v>9.4583084916105953E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:49">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -5433,13 +7636,13 @@
         <f t="shared" si="0"/>
         <v>17628</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="21">
         <v>9808</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="21">
         <v>4868</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="21">
         <v>14676</v>
       </c>
       <c r="H10" s="6">
@@ -5458,10 +7661,10 @@
       <c r="O10" s="10">
         <v>19681</v>
       </c>
-      <c r="P10" s="28">
+      <c r="P10" s="22">
         <v>7845</v>
       </c>
-      <c r="Q10" s="28">
+      <c r="Q10" s="22">
         <v>25945</v>
       </c>
       <c r="R10" s="11">
@@ -5551,7 +7754,7 @@
         <v>8.8002346729246117E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:49">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -5565,13 +7768,13 @@
         <f t="shared" si="0"/>
         <v>17895</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="21">
         <v>10111</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="21">
         <v>4967</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="21">
         <v>15078</v>
       </c>
       <c r="H11" s="6">
@@ -5590,10 +7793,10 @@
       <c r="O11" s="10">
         <v>20988</v>
       </c>
-      <c r="P11" s="28">
+      <c r="P11" s="22">
         <v>8500</v>
       </c>
-      <c r="Q11" s="28">
+      <c r="Q11" s="22">
         <v>27750</v>
       </c>
       <c r="R11" s="11">
@@ -5683,7 +7886,7 @@
         <v>8.7311251826595229E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:49">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -5697,13 +7900,13 @@
         <f t="shared" si="0"/>
         <v>17981</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="21">
         <v>10134</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="21">
         <v>5073</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="21">
         <v>15207</v>
       </c>
       <c r="H12" s="6">
@@ -5722,10 +7925,10 @@
       <c r="O12" s="10">
         <v>22295</v>
       </c>
-      <c r="P12" s="27">
+      <c r="P12" s="21">
         <v>9498</v>
       </c>
-      <c r="Q12" s="27">
+      <c r="Q12" s="21">
         <v>29798</v>
       </c>
       <c r="R12" s="11">
@@ -5815,7 +8018,7 @@
         <v>9.2401892568883939E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:49">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -5829,13 +8032,13 @@
         <f t="shared" si="0"/>
         <v>18579</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="21">
         <v>10198</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="21">
         <v>5278</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="21">
         <v>15476</v>
       </c>
       <c r="H13" s="6">
@@ -5854,10 +8057,10 @@
       <c r="O13" s="10">
         <v>23513</v>
       </c>
-      <c r="P13" s="27">
+      <c r="P13" s="21">
         <v>9880</v>
       </c>
-      <c r="Q13" s="27">
+      <c r="Q13" s="21">
         <v>31880</v>
       </c>
       <c r="R13" s="6">
@@ -5947,7 +8150,7 @@
         <v>0.10144927536231885</v>
       </c>
     </row>
-    <row r="14" spans="1:49">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -5961,13 +8164,13 @@
         <f t="shared" si="0"/>
         <v>18430</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="21">
         <v>10370</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="21">
         <v>5225</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="21">
         <v>15595</v>
       </c>
       <c r="H14" s="6">
@@ -5986,10 +8189,10 @@
       <c r="O14" s="10">
         <v>25280</v>
       </c>
-      <c r="P14" s="27">
+      <c r="P14" s="21">
         <v>10836</v>
       </c>
-      <c r="Q14" s="27">
+      <c r="Q14" s="21">
         <v>33782</v>
       </c>
       <c r="R14" s="6">
@@ -6079,7 +8282,7 @@
         <v>0.12666405638214565</v>
       </c>
     </row>
-    <row r="15" spans="1:49">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -6093,13 +8296,13 @@
         <f t="shared" si="0"/>
         <v>18503</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="21">
         <v>10592</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="21">
         <v>5170</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="21">
         <v>15762</v>
       </c>
       <c r="H15" s="6">
@@ -6118,10 +8321,10 @@
       <c r="O15" s="10">
         <v>26834</v>
       </c>
-      <c r="P15" s="27">
+      <c r="P15" s="21">
         <v>11794</v>
       </c>
-      <c r="Q15" s="27">
+      <c r="Q15" s="21">
         <v>36788</v>
       </c>
       <c r="R15" s="12">
@@ -6211,7 +8414,7 @@
         <v>0.1687463782113193</v>
       </c>
     </row>
-    <row r="16" spans="1:49">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -6225,13 +8428,13 @@
         <f t="shared" si="0"/>
         <v>18370</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="21">
         <v>10518</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="21">
         <v>5304</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="21">
         <v>15822</v>
       </c>
       <c r="H16" s="6">
@@ -6250,10 +8453,10 @@
       <c r="O16" s="10">
         <v>28442</v>
       </c>
-      <c r="P16" s="27">
+      <c r="P16" s="21">
         <v>12224</v>
       </c>
-      <c r="Q16" s="27">
+      <c r="Q16" s="21">
         <v>38236</v>
       </c>
       <c r="R16" s="6">
@@ -6343,7 +8546,7 @@
         <v>0.19193761154651975</v>
       </c>
     </row>
-    <row r="17" spans="1:47">
+    <row r="17" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -6357,13 +8560,13 @@
         <f t="shared" si="0"/>
         <v>18350</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="21">
         <v>10754</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F17" s="21">
         <v>5332</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="21">
         <v>16086</v>
       </c>
       <c r="H17" s="6">
@@ -6382,10 +8585,10 @@
       <c r="O17" s="10">
         <v>30122</v>
       </c>
-      <c r="P17" s="27">
+      <c r="P17" s="21">
         <v>12676</v>
       </c>
-      <c r="Q17" s="27">
+      <c r="Q17" s="21">
         <v>40062</v>
       </c>
       <c r="R17" s="6">
@@ -6475,7 +8678,7 @@
         <v>0.23374821779507535</v>
       </c>
     </row>
-    <row r="18" spans="1:47">
+    <row r="18" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -6489,13 +8692,13 @@
         <f t="shared" si="0"/>
         <v>18415</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="21">
         <v>11021</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="21">
         <v>5462</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="21">
         <v>16483</v>
       </c>
       <c r="H18" s="6">
@@ -6514,10 +8717,10 @@
       <c r="O18" s="10">
         <v>33687</v>
       </c>
-      <c r="P18" s="27">
+      <c r="P18" s="21">
         <v>13216</v>
       </c>
-      <c r="Q18" s="27">
+      <c r="Q18" s="21">
         <v>42402</v>
       </c>
       <c r="R18" s="6">
@@ -6607,7 +8810,7 @@
         <v>0.24161321241613212</v>
       </c>
     </row>
-    <row r="19" spans="1:47">
+    <row r="19" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>68</v>
       </c>
@@ -6621,13 +8824,13 @@
         <f t="shared" si="0"/>
         <v>18523</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E19" s="21">
         <v>11234</v>
       </c>
-      <c r="F19" s="27">
+      <c r="F19" s="21">
         <v>5502</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="21">
         <v>16736</v>
       </c>
       <c r="H19" s="6">
@@ -6646,10 +8849,10 @@
       <c r="O19" s="10">
         <v>33673</v>
       </c>
-      <c r="P19" s="27">
+      <c r="P19" s="21">
         <v>14686</v>
       </c>
-      <c r="Q19" s="27">
+      <c r="Q19" s="21">
         <v>43982</v>
       </c>
       <c r="R19" s="6">
@@ -6739,7 +8942,7 @@
         <v>0.2442537096304917</v>
       </c>
     </row>
-    <row r="20" spans="1:47">
+    <row r="20" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -6753,13 +8956,13 @@
         <f t="shared" si="0"/>
         <v>18862</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="21">
         <v>11361</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F20" s="21">
         <v>4970</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="21">
         <v>16331</v>
       </c>
       <c r="H20" s="6">
@@ -6778,10 +8981,10 @@
       <c r="O20" s="10">
         <v>33916</v>
       </c>
-      <c r="P20" s="27">
+      <c r="P20" s="21">
         <v>15932</v>
       </c>
-      <c r="Q20" s="27">
+      <c r="Q20" s="21">
         <v>45276</v>
       </c>
       <c r="R20" s="6">
@@ -6871,36 +9074,308 @@
         <v>0.24385833219598743</v>
       </c>
     </row>
-    <row r="28" spans="1:47" ht="17">
-      <c r="O28" s="26"/>
-    </row>
-    <row r="30" spans="1:47" ht="16">
-      <c r="E30" s="31"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-    </row>
-    <row r="31" spans="1:47" ht="16">
-      <c r="E31" s="31"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-    </row>
-    <row r="32" spans="1:47" ht="16">
-      <c r="E32" s="31"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-    </row>
-    <row r="33" spans="5:7" ht="16">
-      <c r="E33" s="31"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-    </row>
-    <row r="34" spans="5:7" ht="16">
-      <c r="E34" s="31"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
+    <row r="28" spans="1:52" ht="18" x14ac:dyDescent="0.2">
+      <c r="O28" s="20"/>
+      <c r="AX28" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="AX29" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="AY29" t="s">
+        <v>88</v>
+      </c>
+      <c r="AZ29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="E30" s="25"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="AX30" s="14">
+        <v>0.45809234227834555</v>
+      </c>
+      <c r="AY30" s="3">
+        <v>0.58683196155462591</v>
+      </c>
+      <c r="AZ30">
+        <v>0.26192506916882274</v>
+      </c>
+    </row>
+    <row r="31" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="E31" s="25"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="W31" t="s">
+        <v>97</v>
+      </c>
+      <c r="AX31" s="14">
+        <v>0.45631710947990539</v>
+      </c>
+      <c r="AY31" s="3">
+        <v>0.62142177664070997</v>
+      </c>
+      <c r="AZ31">
+        <v>0.24678900252380159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="E32" s="25"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="W32" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="X32" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>93</v>
+      </c>
+      <c r="AX32" s="14">
+        <v>0.45440487313852768</v>
+      </c>
+      <c r="AY32" s="3">
+        <v>0.61594260376646026</v>
+      </c>
+      <c r="AZ32">
+        <v>0.24217171758594896</v>
+      </c>
+    </row>
+    <row r="33" spans="5:52" x14ac:dyDescent="0.2">
+      <c r="E33" s="25"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="W33" s="14">
+        <v>0.17478392898855408</v>
+      </c>
+      <c r="X33" s="3">
+        <v>0.29733342714416378</v>
+      </c>
+      <c r="Y33" s="3">
+        <v>9.4583084916105953E-2</v>
+      </c>
+      <c r="AX33" s="14">
+        <v>0.46667584747115842</v>
+      </c>
+      <c r="AY33" s="3">
+        <v>0.61097116035856824</v>
+      </c>
+      <c r="AZ33">
+        <v>0.25189891935540981</v>
+      </c>
+    </row>
+    <row r="34" spans="5:52" x14ac:dyDescent="0.2">
+      <c r="E34" s="25"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="W34" s="14">
+        <v>0.17670751077830724</v>
+      </c>
+      <c r="X34" s="3">
+        <v>0.33169801035704549</v>
+      </c>
+      <c r="Y34" s="3">
+        <v>8.8002346729246117E-2</v>
+      </c>
+      <c r="AX34" s="14">
+        <v>0.48962339387579235</v>
+      </c>
+      <c r="AY34" s="3">
+        <v>0.62546777386033281</v>
+      </c>
+      <c r="AZ34">
+        <v>0.26530436722110062</v>
+      </c>
+    </row>
+    <row r="35" spans="5:52" x14ac:dyDescent="0.2">
+      <c r="W35" s="14">
+        <v>0.17485331098072088</v>
+      </c>
+      <c r="X35" s="3">
+        <v>0.32942034752619709</v>
+      </c>
+      <c r="Y35" s="3">
+        <v>8.7311251826595229E-2</v>
+      </c>
+      <c r="AX35" s="14">
+        <v>0.47390653258829013</v>
+      </c>
+      <c r="AY35" s="3">
+        <v>0.61101767178492317</v>
+      </c>
+      <c r="AZ35">
+        <v>0.29144090280858503</v>
+      </c>
+    </row>
+    <row r="36" spans="5:52" x14ac:dyDescent="0.2">
+      <c r="W36" s="14">
+        <v>0.1747956175963517</v>
+      </c>
+      <c r="X36" s="3">
+        <v>0.33359637009272047</v>
+      </c>
+      <c r="Y36" s="33">
+        <v>9.2401892568883939E-2</v>
+      </c>
+      <c r="AX36" s="14">
+        <v>0.48064358456906631</v>
+      </c>
+      <c r="AY36" s="3">
+        <v>0.60356806754165282</v>
+      </c>
+      <c r="AZ36">
+        <v>0.34390640543038581</v>
+      </c>
+    </row>
+    <row r="37" spans="5:52" x14ac:dyDescent="0.2">
+      <c r="W37" s="14">
+        <v>0.18666236072985629</v>
+      </c>
+      <c r="X37" s="3">
+        <v>0.34104419746704573</v>
+      </c>
+      <c r="Y37" s="3">
+        <v>0.10144927536231885</v>
+      </c>
+      <c r="AX37" s="14">
+        <v>0.46819773200174103</v>
+      </c>
+      <c r="AY37" s="3">
+        <v>0.61200533861594031</v>
+      </c>
+      <c r="AZ37">
+        <v>0.37506123354719134</v>
+      </c>
+    </row>
+    <row r="38" spans="5:52" x14ac:dyDescent="0.2">
+      <c r="W38" s="14">
+        <v>0.1919153553988063</v>
+      </c>
+      <c r="X38" s="3">
+        <v>0.33504328310355885</v>
+      </c>
+      <c r="Y38" s="3">
+        <v>0.12666405638214565</v>
+      </c>
+      <c r="AX38" s="14">
+        <v>0.46349421265426177</v>
+      </c>
+      <c r="AY38" s="3">
+        <v>0.61044102842008585</v>
+      </c>
+      <c r="AZ38">
+        <v>0.43296257539942906</v>
+      </c>
+    </row>
+    <row r="39" spans="5:52" x14ac:dyDescent="0.2">
+      <c r="W39" s="14">
+        <v>0.1946711344106361</v>
+      </c>
+      <c r="X39" s="3">
+        <v>0.32800406039842661</v>
+      </c>
+      <c r="Y39" s="3">
+        <v>0.1687463782113193</v>
+      </c>
+      <c r="AX39" s="14">
+        <v>0.49029438157013605</v>
+      </c>
+      <c r="AY39" s="3">
+        <v>0.61391046428598128</v>
+      </c>
+      <c r="AZ39">
+        <v>0.44086479375197685</v>
+      </c>
+    </row>
+    <row r="40" spans="5:52" x14ac:dyDescent="0.2">
+      <c r="W40" s="14">
+        <v>0.19227000544365813</v>
+      </c>
+      <c r="X40" s="3">
+        <v>0.33522942737959804</v>
+      </c>
+      <c r="Y40" s="3">
+        <v>0.19193761154651975</v>
+      </c>
+      <c r="AX40" s="14">
+        <v>0.47474976056672163</v>
+      </c>
+      <c r="AY40" s="3">
+        <v>0.5946091338958861</v>
+      </c>
+      <c r="AZ40">
+        <v>0.44781713241174109</v>
+      </c>
+    </row>
+    <row r="41" spans="5:52" x14ac:dyDescent="0.2">
+      <c r="W41" s="14">
+        <v>0.19302452316076293</v>
+      </c>
+      <c r="X41" s="3">
+        <v>0.33146835757801818</v>
+      </c>
+      <c r="Y41" s="3">
+        <v>0.23374821779507535</v>
+      </c>
+      <c r="AX41" s="14">
+        <v>0.45550802626141568</v>
+      </c>
+      <c r="AY41" s="3">
+        <v>0.55420632886278287</v>
+      </c>
+      <c r="AZ41">
+        <v>0.45783237515159092</v>
+      </c>
+    </row>
+    <row r="42" spans="5:52" x14ac:dyDescent="0.2">
+      <c r="W42" s="14">
+        <v>0.19245180559326636</v>
+      </c>
+      <c r="X42" s="3">
+        <v>0.33137171631377782</v>
+      </c>
+      <c r="Y42" s="3">
+        <v>0.24161321241613212</v>
+      </c>
+    </row>
+    <row r="43" spans="5:52" x14ac:dyDescent="0.2">
+      <c r="W43" s="14">
+        <v>0.187388651946229</v>
+      </c>
+      <c r="X43" s="3">
+        <v>0.3287523900573614</v>
+      </c>
+      <c r="Y43" s="3">
+        <v>0.2442537096304917</v>
+      </c>
+    </row>
+    <row r="44" spans="5:52" x14ac:dyDescent="0.2">
+      <c r="W44" s="14">
+        <v>0.17893118439189906</v>
+      </c>
+      <c r="X44" s="3">
+        <v>0.30432918988426916</v>
+      </c>
+      <c r="Y44" s="3">
+        <v>0.24385833219598743</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:AG1"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="AB2:AD2"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="AP1:AW1"/>
     <mergeCell ref="AP2:AQ2"/>
@@ -6917,23 +9392,9 @@
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:AG1"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="AB2:AD2"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:U2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>